<commit_message>
add biginteger and word
</commit_message>
<xml_diff>
--- a/论文/timedata.xlsx
+++ b/论文/timedata.xlsx
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -835,7 +835,88 @@
         <v>-6.2465836585876695E+18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16">
+        <f>SUM(B6:B8)/3</f>
+        <v>577718143.66666663</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C6:C8)/3</f>
+        <v>76620</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="C16:H17" si="0">SUM(D6:D8)/3</f>
+        <v>22593</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2463</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>1464</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>6568.666666666667</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>2038.3333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C17">
+        <f>SUM(C9:C11)/3</f>
+        <v>104838.33333333333</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:H17" si="1">SUM(D9:D11)/3</f>
+        <v>34416.666666666664</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>3215.6666666666665</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>2394.6666666666665</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>7348.333333333333</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>2093.3333333333335</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C18">
+        <f>SUM(C12:C14)/3</f>
+        <v>111393</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:H18" si="2">SUM(D12:D14)/3</f>
+        <v>44023</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>3448.3333333333335</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>2722.6666666666665</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>10687.333333333334</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>2025</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>